<commit_message>
All Datatables updated. MTR366 added.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/GOC.xlsx
+++ b/src/test/resources/testdata/GOC.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20400"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3F1472-000D-4AB7-9991-4345E85E846F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6310AE-3F29-4D30-8D45-825831BD75A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,9 +58,6 @@
     <t>1163 Oak Bluff Dr</t>
   </si>
   <si>
-    <t>07302023</t>
-  </si>
-  <si>
     <t>Florida</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
   </si>
   <si>
     <t>$1,000</t>
+  </si>
+  <si>
+    <t>08152023</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,19 +479,19 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -511,63 +511,63 @@
         <v>33837</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="K2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="K3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>